<commit_message>
Removed some magic numbers; added downloading newest data feature; started prep for visualization more than temperature; made pre-PoC of web app
</commit_message>
<xml_diff>
--- a/bands_excel.xlsx
+++ b/bands_excel.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuba\Desktop\Projekt_GFS\GFS-forecast-web-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBF62B39-B675-4CEE-B14C-CBBD7D4CE426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1FC73D-3FE4-4018-A66E-AAEDC6467645}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bands" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="135">
   <si>
     <t>Cloud mixing ratio [kg/kg]</t>
   </si>
@@ -430,7 +431,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -585,7 +586,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -765,6 +766,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -926,8 +939,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% — akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1282,16 +1298,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E521"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146:C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.109375" customWidth="1"/>
     <col min="3" max="3" width="35.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1412,7 +1428,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>11</v>
       </c>
       <c r="B11" t="s">
@@ -2875,7 +2891,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144">
+      <c r="A144" s="3">
         <v>144</v>
       </c>
       <c r="B144" t="s">
@@ -2886,7 +2902,7 @@
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145">
+      <c r="A145" s="3">
         <v>145</v>
       </c>
       <c r="B145" t="s">
@@ -2897,7 +2913,7 @@
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146">
+      <c r="A146" s="1">
         <v>146</v>
       </c>
       <c r="B146" t="s">
@@ -2908,7 +2924,7 @@
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147">
+      <c r="A147" s="1">
         <v>147</v>
       </c>
       <c r="B147" t="s">
@@ -5719,7 +5735,7 @@
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A402">
+      <c r="A402" s="3">
         <v>402</v>
       </c>
       <c r="B402" t="s">
@@ -5862,7 +5878,7 @@
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A415">
+      <c r="A415" s="1">
         <v>415</v>
       </c>
       <c r="B415" t="s">
@@ -5884,7 +5900,7 @@
       </c>
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A417">
+      <c r="A417" s="1">
         <v>417</v>
       </c>
       <c r="B417" t="s">
@@ -5923,7 +5939,7 @@
       </c>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A420">
+      <c r="A420" s="1">
         <v>420</v>
       </c>
       <c r="B420" t="s">
@@ -5934,7 +5950,7 @@
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A421">
+      <c r="A421" s="1">
         <v>421</v>
       </c>
       <c r="B421" t="s">
@@ -5967,7 +5983,7 @@
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A424">
+      <c r="A424" s="1">
         <v>424</v>
       </c>
       <c r="B424" t="s">
@@ -6043,7 +6059,7 @@
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A432">
+      <c r="A432" s="1">
         <v>432</v>
       </c>
       <c r="B432" t="s">
@@ -6054,7 +6070,7 @@
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A433">
+      <c r="A433" s="2">
         <v>433</v>
       </c>
       <c r="B433" t="s">
@@ -6065,7 +6081,7 @@
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A434">
+      <c r="A434" s="1">
         <v>434</v>
       </c>
       <c r="B434" t="s">
@@ -7008,7 +7024,7 @@
       </c>
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A520">
+      <c r="A520" s="1">
         <v>520</v>
       </c>
       <c r="B520" t="s">
@@ -7027,6 +7043,158 @@
       </c>
       <c r="C521" t="s">
         <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26ACF585-AAA2-494A-A909-41F40D08BA45}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="43.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>415</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>417</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>420</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>421</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>424</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>432</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>433</v>
+      </c>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>434</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>520</v>
+      </c>
+      <c r="B12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>